<commit_message>
Johns: corrected typo in vin upload spreadsheet
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/VinUploadOnCurrentTerm.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/VinUploadOnCurrentTerm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gw3eraj\projects\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Documents\CSAA\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -323,9 +323,6 @@
     <t>O</t>
   </si>
   <si>
-    <t>2HNYD2H6%C</t>
-  </si>
-  <si>
     <t>ACUR</t>
   </si>
   <si>
@@ -347,9 +344,6 @@
     <t>K</t>
   </si>
   <si>
-    <t>5YMGY0C5%A</t>
-  </si>
-  <si>
     <t>BMW</t>
   </si>
   <si>
@@ -363,6 +357,12 @@
   </si>
   <si>
     <t>4.4L V8 TURBO</t>
+  </si>
+  <si>
+    <t>2HNYD2H6&amp;C</t>
+  </si>
+  <si>
+    <t>5YMGY0C5&amp;A</t>
   </si>
 </sst>
 </file>
@@ -725,29 +725,29 @@
   <dimension ref="A1:AJ8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A7" sqref="A7:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.77734375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -857,7 +857,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -958,7 +958,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>66</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>76</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1364,9 +1364,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>65</v>
@@ -1375,16 +1375,16 @@
         <v>2012</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>103</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>47</v>
@@ -1402,13 +1402,13 @@
         <v>49</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O7" s="6">
         <v>6</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S7" s="6">
         <v>4</v>
@@ -1441,16 +1441,16 @@
         <v>38</v>
       </c>
       <c r="AC7" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AD7" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AE7" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AF7" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AG7" s="4">
         <v>20180709</v>
@@ -1465,9 +1465,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>65</v>
@@ -1476,16 +1476,16 @@
         <v>2010</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="G8" t="s">
         <v>109</v>
-      </c>
-      <c r="F8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G8" t="s">
-        <v>111</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>47</v>
@@ -1503,13 +1503,13 @@
         <v>49</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="O8" s="3">
         <v>8</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S8" s="3">
         <v>4</v>
@@ -1542,16 +1542,16 @@
         <v>38</v>
       </c>
       <c r="AC8" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AD8" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AE8" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AF8" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AG8" s="4">
         <v>20180709</v>

</xml_diff>

<commit_message>
Fixed changes for PAS-14532-Current Term End Adds Vehicle: make refresh correct for current and renewal terms
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/VinUploadOnCurrentTerm.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/VinUploadOnCurrentTerm.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="120">
   <si>
     <t>VIN</t>
   </si>
@@ -323,9 +323,6 @@
     <t>O</t>
   </si>
   <si>
-    <t>2HNYD2H6%C</t>
-  </si>
-  <si>
     <t>ACUR</t>
   </si>
   <si>
@@ -347,22 +344,46 @@
     <t>K</t>
   </si>
   <si>
-    <t>5YMGY0C5%A</t>
-  </si>
-  <si>
     <t>BMW</t>
   </si>
   <si>
     <t xml:space="preserve">BMW MOTOR </t>
   </si>
   <si>
-    <t>X5</t>
-  </si>
-  <si>
-    <t>X5 M</t>
-  </si>
-  <si>
-    <t>4.4L V8 TURBO</t>
+    <t>SYMBOL_2018_CHOICE</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>2HNYD2H6&amp;C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>WBSAK031%M</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>2D CPE</t>
+  </si>
+  <si>
+    <t>SEDAN 2 DOOR</t>
+  </si>
+  <si>
+    <t>CPE</t>
+  </si>
+  <si>
+    <t>2.3L L4</t>
+  </si>
+  <si>
+    <t>000M</t>
+  </si>
+  <si>
+    <t>DRIVER ONLY AIRBAG</t>
   </si>
 </sst>
 </file>
@@ -722,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ8"/>
+  <dimension ref="A1:AJ15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -857,7 +878,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -958,45 +979,45 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="C3" s="3">
-        <v>1991</v>
+        <v>2010</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O3" s="3">
         <v>4</v>
@@ -1007,29 +1028,29 @@
       <c r="S3" s="3">
         <v>2</v>
       </c>
-      <c r="T3" s="3" t="s">
-        <v>54</v>
+      <c r="T3" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="U3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="V3" s="3">
-        <v>1</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>57</v>
+        <v>2</v>
+      </c>
+      <c r="W3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" s="3">
+        <v>2</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="Z3" s="3">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="AA3" s="3">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="AB3" s="3" t="s">
         <v>38</v>
@@ -1059,93 +1080,93 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="1:36" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="6">
-        <v>2000</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="O4" s="6">
-        <v>6</v>
-      </c>
-      <c r="R4" s="6" t="s">
+      <c r="C4" s="3">
+        <v>1991</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="3">
+        <v>4</v>
+      </c>
+      <c r="R4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S4" s="6">
-        <v>2</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="V4" s="6">
-        <v>2</v>
-      </c>
-      <c r="W4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="X4" s="6" t="s">
+      <c r="S4" s="3">
+        <v>2</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U4" t="s">
+        <v>55</v>
+      </c>
+      <c r="V4" s="3">
+        <v>1</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="Y4" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z4" s="6">
-        <v>37</v>
-      </c>
-      <c r="AA4" s="6">
-        <v>25</v>
+      <c r="Y4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>30</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>20</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AC4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AE4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AF4" s="6" t="s">
-        <v>84</v>
+      <c r="AC4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="AG4" s="4">
         <v>20180709</v>
@@ -1160,93 +1181,93 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="6">
-        <v>2009</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="I5" s="6" t="s">
+    <row r="5" spans="1:36" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1991</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="L5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="O5" s="6">
+      <c r="N5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" s="3">
         <v>4</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="R5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S5" s="6">
-        <v>2</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="V5" s="6">
-        <v>2</v>
-      </c>
-      <c r="W5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="X5" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y5" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z5" s="6">
-        <v>17</v>
-      </c>
-      <c r="AA5" s="6">
-        <v>12</v>
+      <c r="S5" s="3">
+        <v>2</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U5" t="s">
+        <v>55</v>
+      </c>
+      <c r="V5" s="3">
+        <v>1</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>6</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>6</v>
       </c>
       <c r="AB5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AC5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF5" s="6" t="s">
-        <v>38</v>
+      <c r="AC5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="AG5" s="4">
         <v>20180709</v>
@@ -1261,61 +1282,59 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>87</v>
+    <row r="6" spans="1:36" s="6" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C6" s="6">
-        <v>2003</v>
-      </c>
-      <c r="D6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" t="s">
-        <v>89</v>
-      </c>
-      <c r="F6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G6" t="s">
-        <v>91</v>
-      </c>
-      <c r="I6" t="s">
-        <v>92</v>
-      </c>
-      <c r="J6" t="s">
-        <v>93</v>
-      </c>
-      <c r="K6" t="s">
-        <v>93</v>
-      </c>
-      <c r="L6" t="s">
-        <v>93</v>
-      </c>
-      <c r="M6" t="s">
-        <v>94</v>
-      </c>
-      <c r="N6" t="s">
-        <v>95</v>
+        <v>2000</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="O6" s="6">
-        <v>8</v>
-      </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
+        <v>6</v>
+      </c>
       <c r="R6" s="6" t="s">
         <v>36</v>
       </c>
       <c r="S6" s="6">
         <v>2</v>
       </c>
-      <c r="T6" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="U6" t="s">
+      <c r="T6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="U6" s="6" t="s">
         <v>74</v>
       </c>
       <c r="V6" s="6">
@@ -1325,31 +1344,31 @@
         <v>37</v>
       </c>
       <c r="X6" s="6" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="Y6" s="6" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="Z6" s="6">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="AA6" s="6">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="AB6" s="3" t="s">
         <v>38</v>
       </c>
       <c r="AC6" s="6" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="AD6" s="6" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="AE6" s="6" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="AF6" s="6" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="AG6" s="4">
         <v>20180709</v>
@@ -1364,60 +1383,60 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" s="6" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="C7" s="6">
-        <v>2012</v>
+        <v>2000</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>49</v>
+        <v>69</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="O7" s="6">
         <v>6</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>105</v>
+        <v>36</v>
       </c>
       <c r="S7" s="6">
-        <v>4</v>
-      </c>
-      <c r="T7" s="5" t="s">
-        <v>58</v>
+        <v>2</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="V7" s="6">
         <v>2</v>
@@ -1426,31 +1445,31 @@
         <v>37</v>
       </c>
       <c r="X7" s="6" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="Y7" s="6" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="Z7" s="6">
         <v>13</v>
       </c>
       <c r="AA7" s="6">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AB7" s="3" t="s">
         <v>38</v>
       </c>
       <c r="AC7" s="6" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="AD7" s="6" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="AE7" s="6" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="AF7" s="6" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="AG7" s="4">
         <v>20180709</v>
@@ -1465,93 +1484,93 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:36" s="6" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="3">
-        <v>2010</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G8" t="s">
-        <v>111</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="O8" s="3">
-        <v>8</v>
+      <c r="C8" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="O8" s="6">
+        <v>4</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="S8" s="3">
-        <v>4</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="U8" t="s">
+        <v>36</v>
+      </c>
+      <c r="S8" s="6">
+        <v>2</v>
+      </c>
+      <c r="T8" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="U8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="V8" s="3">
-        <v>2</v>
-      </c>
-      <c r="W8" t="s">
+      <c r="V8" s="6">
+        <v>2</v>
+      </c>
+      <c r="W8" s="6" t="s">
         <v>37</v>
       </c>
       <c r="X8" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="Y8" s="3" t="s">
+      <c r="Y8" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="Z8" s="3">
-        <v>60</v>
-      </c>
-      <c r="AA8" s="3">
-        <v>32</v>
+      <c r="Z8" s="6">
+        <v>17</v>
+      </c>
+      <c r="AA8" s="6">
+        <v>12</v>
       </c>
       <c r="AB8" s="3" t="s">
         <v>38</v>
       </c>
       <c r="AC8" s="6" t="s">
-        <v>106</v>
+        <v>38</v>
       </c>
       <c r="AD8" s="6" t="s">
-        <v>106</v>
+        <v>38</v>
       </c>
       <c r="AE8" s="6" t="s">
-        <v>106</v>
+        <v>38</v>
       </c>
       <c r="AF8" s="6" t="s">
-        <v>106</v>
+        <v>38</v>
       </c>
       <c r="AG8" s="4">
         <v>20180709</v>
@@ -1563,6 +1582,717 @@
         <v>38</v>
       </c>
       <c r="AJ8" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" s="6" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="O9" s="6">
+        <v>4</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S9" s="6">
+        <v>2</v>
+      </c>
+      <c r="T9" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="U9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V9" s="6">
+        <v>2</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="X9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y9" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>20</v>
+      </c>
+      <c r="AA9" s="6">
+        <v>20</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG9" s="4">
+        <v>20180709</v>
+      </c>
+      <c r="AH9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ9" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="6">
+        <v>2003</v>
+      </c>
+      <c r="D10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" t="s">
+        <v>91</v>
+      </c>
+      <c r="I10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" t="s">
+        <v>93</v>
+      </c>
+      <c r="K10" t="s">
+        <v>93</v>
+      </c>
+      <c r="L10" t="s">
+        <v>93</v>
+      </c>
+      <c r="M10" t="s">
+        <v>94</v>
+      </c>
+      <c r="N10" t="s">
+        <v>95</v>
+      </c>
+      <c r="O10" s="6">
+        <v>8</v>
+      </c>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S10" s="6">
+        <v>2</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="U10" t="s">
+        <v>74</v>
+      </c>
+      <c r="V10" s="6">
+        <v>2</v>
+      </c>
+      <c r="W10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="X10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y10" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z10" s="6">
+        <v>50</v>
+      </c>
+      <c r="AA10" s="6">
+        <v>50</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG10" s="4">
+        <v>20180709</v>
+      </c>
+      <c r="AH10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ10" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="6">
+        <v>2003</v>
+      </c>
+      <c r="D11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" t="s">
+        <v>93</v>
+      </c>
+      <c r="K11" t="s">
+        <v>93</v>
+      </c>
+      <c r="L11" t="s">
+        <v>93</v>
+      </c>
+      <c r="M11" t="s">
+        <v>94</v>
+      </c>
+      <c r="N11" t="s">
+        <v>95</v>
+      </c>
+      <c r="O11" s="6">
+        <v>8</v>
+      </c>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S11" s="6">
+        <v>2</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="U11" t="s">
+        <v>74</v>
+      </c>
+      <c r="V11" s="6">
+        <v>2</v>
+      </c>
+      <c r="W11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="X11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y11" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z11" s="6">
+        <v>77</v>
+      </c>
+      <c r="AA11" s="6">
+        <v>77</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC11" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD11" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE11" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF11" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AG11" s="4">
+        <v>20180709</v>
+      </c>
+      <c r="AH11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ11" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" s="6" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="6">
+        <v>2012</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="O12" s="6">
+        <v>6</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="S12" s="6">
+        <v>4</v>
+      </c>
+      <c r="T12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="U12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V12" s="6">
+        <v>2</v>
+      </c>
+      <c r="W12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="X12" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y12" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z12" s="6">
+        <v>13</v>
+      </c>
+      <c r="AA12" s="6">
+        <v>16</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC12" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD12" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE12" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF12" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AG12" s="4">
+        <v>20180709</v>
+      </c>
+      <c r="AH12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ12" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" s="6" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2012</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="O13" s="6">
+        <v>6</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="S13" s="6">
+        <v>4</v>
+      </c>
+      <c r="T13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="U13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V13" s="6">
+        <v>2</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="X13" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y13" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z13" s="6">
+        <v>33</v>
+      </c>
+      <c r="AA13" s="6">
+        <v>33</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC13" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD13" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE13" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF13" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AG13" s="4">
+        <v>20180709</v>
+      </c>
+      <c r="AH13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ13" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1991</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G14" t="s">
+        <v>113</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K14" t="s">
+        <v>115</v>
+      </c>
+      <c r="L14" t="s">
+        <v>115</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="N14" t="s">
+        <v>117</v>
+      </c>
+      <c r="O14" s="6">
+        <v>4</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S14" s="6">
+        <v>2</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="U14" t="s">
+        <v>119</v>
+      </c>
+      <c r="V14" s="6">
+        <v>2</v>
+      </c>
+      <c r="W14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="X14" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y14" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z14" s="6">
+        <v>12</v>
+      </c>
+      <c r="AA14" s="6">
+        <v>12</v>
+      </c>
+      <c r="AB14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC14" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AD14" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE14" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF14" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AG14" s="4">
+        <v>20180709</v>
+      </c>
+      <c r="AH14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ14" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1991</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" t="s">
+        <v>113</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K15" t="s">
+        <v>115</v>
+      </c>
+      <c r="L15" t="s">
+        <v>115</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="N15" t="s">
+        <v>117</v>
+      </c>
+      <c r="O15" s="6">
+        <v>4</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S15" s="6">
+        <v>2</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="U15" t="s">
+        <v>119</v>
+      </c>
+      <c r="V15" s="6">
+        <v>2</v>
+      </c>
+      <c r="W15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="X15" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y15" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z15" s="6">
+        <v>7</v>
+      </c>
+      <c r="AA15" s="6">
+        <v>7</v>
+      </c>
+      <c r="AB15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC15" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AD15" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE15" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF15" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AG15" s="4">
+        <v>20180709</v>
+      </c>
+      <c r="AH15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ15" s="4" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Johns: Conflict Page Changes are added
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/VinUploadOnCurrentTerm.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/VinUploadOnCurrentTerm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gw3eraj\projects\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Documents\CSAA\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -362,9 +362,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>WBSAK031%M</t>
-  </si>
-  <si>
     <t>M3</t>
   </si>
   <si>
@@ -384,6 +381,9 @@
   </si>
   <si>
     <t>DRIVER ONLY AIRBAG</t>
+  </si>
+  <si>
+    <t>WBSAK031&amp;M</t>
   </si>
 </sst>
 </file>
@@ -746,29 +746,29 @@
   <dimension ref="A1:AJ15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.77734375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -878,7 +878,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -979,7 +979,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:36" s="6" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" s="6" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>66</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:36" s="6" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" s="6" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>66</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:36" s="6" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" s="6" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>76</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:36" s="6" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" s="6" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>76</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:36" s="6" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" s="6" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>110</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:36" s="6" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" s="6" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>110</v>
       </c>
@@ -2094,9 +2094,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>65</v>
@@ -2111,28 +2111,28 @@
         <v>107</v>
       </c>
       <c r="F14" t="s">
+        <v>112</v>
+      </c>
+      <c r="G14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G14" t="s">
-        <v>113</v>
-      </c>
-      <c r="I14" s="3" t="s">
+      <c r="J14" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" t="s">
+        <v>114</v>
+      </c>
+      <c r="L14" t="s">
+        <v>114</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="K14" t="s">
-        <v>115</v>
-      </c>
-      <c r="L14" t="s">
-        <v>115</v>
-      </c>
-      <c r="M14" s="3" t="s">
+      <c r="N14" t="s">
         <v>116</v>
-      </c>
-      <c r="N14" t="s">
-        <v>117</v>
       </c>
       <c r="O14" s="6">
         <v>4</v>
@@ -2144,10 +2144,10 @@
         <v>2</v>
       </c>
       <c r="T14" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="U14" t="s">
         <v>118</v>
-      </c>
-      <c r="U14" t="s">
-        <v>119</v>
       </c>
       <c r="V14" s="6">
         <v>2</v>
@@ -2195,9 +2195,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:36" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>108</v>
@@ -2212,28 +2212,28 @@
         <v>107</v>
       </c>
       <c r="F15" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" t="s">
+        <v>112</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G15" t="s">
-        <v>113</v>
-      </c>
-      <c r="I15" s="3" t="s">
+      <c r="J15" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="K15" t="s">
+        <v>114</v>
+      </c>
+      <c r="L15" t="s">
+        <v>114</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="K15" t="s">
-        <v>115</v>
-      </c>
-      <c r="L15" t="s">
-        <v>115</v>
-      </c>
-      <c r="M15" s="3" t="s">
+      <c r="N15" t="s">
         <v>116</v>
-      </c>
-      <c r="N15" t="s">
-        <v>117</v>
       </c>
       <c r="O15" s="6">
         <v>4</v>
@@ -2245,10 +2245,10 @@
         <v>2</v>
       </c>
       <c r="T15" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="U15" t="s">
         <v>118</v>
-      </c>
-      <c r="U15" t="s">
-        <v>119</v>
       </c>
       <c r="V15" s="6">
         <v>2</v>

</xml_diff>